<commit_message>
Updated dataset and script
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dean/Dropbox/phs_phd/Teaching Fellow/id_529/joining_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0AAA62-4237-5944-9590-5DD68AD635B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0225D2-ED92-C24B-BA6A-FCC9E88CC759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{E3D1875B-0917-E14A-9D2E-FF56EF36D9A8}"/>
+    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{E3D1875B-0917-E14A-9D2E-FF56EF36D9A8}"/>
   </bookViews>
   <sheets>
     <sheet name="id" sheetId="1" r:id="rId1"/>
     <sheet name="sleep" sheetId="2" r:id="rId2"/>
     <sheet name="coffee" sheetId="3" r:id="rId3"/>
     <sheet name="love" sheetId="4" r:id="rId4"/>
+    <sheet name="overview" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="27">
   <si>
     <t>first_name</t>
   </si>
@@ -105,13 +106,28 @@
   </si>
   <si>
     <t>yes!!!!</t>
+  </si>
+  <si>
+    <t>id_df</t>
+  </si>
+  <si>
+    <t>sleep_df</t>
+  </si>
+  <si>
+    <t>coffee_df</t>
+  </si>
+  <si>
+    <t>loveid529_df</t>
+  </si>
+  <si>
+    <t>Dataset name:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,16 +135,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -136,12 +183,120 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA0E248-3921-714F-BD45-0D076410F46F}">
   <dimension ref="B1:C9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView zoomScale="181" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -569,7 +724,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection sqref="A1:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -654,7 +809,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -767,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAB70FC4-06A3-9042-8801-628E867F551A}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K39" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -848,4 +1003,310 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E43C5D-963E-6B45-ACB5-3C015DC26FB5}">
+  <dimension ref="A1:O11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.1640625" customWidth="1"/>
+    <col min="9" max="9" width="3.1640625" customWidth="1"/>
+    <col min="13" max="13" width="3.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13">
+        <v>100</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="1">
+        <v>6.3</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L4" s="1">
+        <v>2</v>
+      </c>
+      <c r="N4" s="15">
+        <v>100</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B5" s="7">
+        <v>2</v>
+      </c>
+      <c r="C5" s="13">
+        <v>200</v>
+      </c>
+      <c r="E5" s="7">
+        <v>2</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1">
+        <v>8.1</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" s="1">
+        <v>2</v>
+      </c>
+      <c r="N5" s="15">
+        <v>200</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B6" s="7">
+        <v>3</v>
+      </c>
+      <c r="C6" s="13">
+        <v>300</v>
+      </c>
+      <c r="E6" s="7">
+        <v>3</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5.4</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" s="1">
+        <v>3</v>
+      </c>
+      <c r="N6" s="15">
+        <v>300</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13">
+        <v>400</v>
+      </c>
+      <c r="E7" s="8">
+        <v>4</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="2">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="1">
+        <v>1</v>
+      </c>
+      <c r="N7" s="15">
+        <v>400</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B8" s="7">
+        <v>5</v>
+      </c>
+      <c r="C8" s="13">
+        <v>500</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="15">
+        <v>500</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B9" s="7">
+        <v>6</v>
+      </c>
+      <c r="C9" s="13">
+        <v>600</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="15">
+        <v>600</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B10" s="7">
+        <v>7</v>
+      </c>
+      <c r="C10" s="13">
+        <v>700</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="L10" s="1">
+        <v>1</v>
+      </c>
+      <c r="N10" s="15">
+        <v>700</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>8</v>
+      </c>
+      <c r="C11" s="14">
+        <v>800</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="N11" s="16">
+        <v>800</v>
+      </c>
+      <c r="O11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added datasets screenshots and made minor updates to README.
</commit_message>
<xml_diff>
--- a/sample_data.xlsx
+++ b/sample_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dean/Dropbox/phs_phd/Teaching Fellow/id_529/joining_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C0225D2-ED92-C24B-BA6A-FCC9E88CC759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96165135-CBB8-8F4C-91AB-8BDD583341C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{E3D1875B-0917-E14A-9D2E-FF56EF36D9A8}"/>
   </bookViews>
@@ -289,7 +289,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1007,302 +1007,304 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E43C5D-963E-6B45-ACB5-3C015DC26FB5}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="B2:Q12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
+      <selection activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.1640625" customWidth="1"/>
-    <col min="9" max="9" width="3.1640625" customWidth="1"/>
-    <col min="13" max="13" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" customWidth="1"/>
+    <col min="6" max="6" width="3.1640625" customWidth="1"/>
+    <col min="11" max="11" width="3.1640625" customWidth="1"/>
+    <col min="15" max="15" width="3.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="E4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="N4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="O3" s="4" t="s">
+      <c r="P4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B4" s="7">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="C4" s="13">
+      <c r="E5" s="13">
         <v>100</v>
       </c>
-      <c r="E4" s="7">
+      <c r="G5" s="7">
         <v>1</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="H5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="I5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="1">
+      <c r="J5" s="1">
         <v>6.3</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="9" t="s">
+      <c r="M5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N5" s="1">
         <v>2</v>
       </c>
-      <c r="N4" s="15">
+      <c r="P5" s="15">
         <v>100</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B5" s="7">
+      <c r="Q5" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D6" s="7">
         <v>2</v>
       </c>
-      <c r="C5" s="13">
+      <c r="E6" s="13">
         <v>200</v>
       </c>
-      <c r="E5" s="7">
+      <c r="G6" s="7">
         <v>2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="H6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="I6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1">
+      <c r="J6" s="1">
         <v>8.1</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="L6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="M6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N6" s="1">
         <v>2</v>
       </c>
-      <c r="N5" s="15">
+      <c r="P6" s="15">
         <v>200</v>
       </c>
-      <c r="O5" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B6" s="7">
+      <c r="Q6" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D7" s="7">
         <v>3</v>
       </c>
-      <c r="C6" s="13">
+      <c r="E7" s="13">
         <v>300</v>
       </c>
-      <c r="E6" s="7">
+      <c r="G7" s="7">
         <v>3</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="I7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="1">
+      <c r="J7" s="1">
         <v>5.4</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="L7" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="M7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N7" s="1">
         <v>3</v>
       </c>
-      <c r="N6" s="15">
+      <c r="P7" s="15">
         <v>300</v>
       </c>
-      <c r="O6" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="Q7" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="7">
         <v>4</v>
       </c>
-      <c r="C7" s="13">
+      <c r="E8" s="13">
         <v>400</v>
       </c>
-      <c r="E7" s="8">
+      <c r="G8" s="8">
         <v>4</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="2">
+      <c r="J8" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="L8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="M8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N8" s="1">
         <v>1</v>
       </c>
-      <c r="N7" s="15">
+      <c r="P8" s="15">
         <v>400</v>
       </c>
-      <c r="O7" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B8" s="7">
+      <c r="Q8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D9" s="7">
         <v>5</v>
       </c>
-      <c r="C8" s="13">
+      <c r="E9" s="13">
         <v>500</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="L9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="M9" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="L8" s="1">
+      <c r="N9" s="1">
         <v>0</v>
       </c>
-      <c r="N8" s="15">
+      <c r="P9" s="15">
         <v>500</v>
       </c>
-      <c r="O8" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B9" s="7">
+      <c r="Q9" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D10" s="7">
         <v>6</v>
       </c>
-      <c r="C9" s="13">
+      <c r="E10" s="13">
         <v>600</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="L10" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="M10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L9" s="1">
+      <c r="N10" s="1">
         <v>0</v>
       </c>
-      <c r="N9" s="15">
+      <c r="P10" s="15">
         <v>600</v>
       </c>
-      <c r="O9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B10" s="7">
+      <c r="Q10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D11" s="7">
         <v>7</v>
       </c>
-      <c r="C10" s="13">
+      <c r="E11" s="13">
         <v>700</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="L11" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="M11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="L10" s="1">
+      <c r="N11" s="1">
         <v>1</v>
       </c>
-      <c r="N10" s="15">
+      <c r="P11" s="15">
         <v>700</v>
       </c>
-      <c r="O10" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="8">
+      <c r="Q11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="8">
         <v>8</v>
       </c>
-      <c r="C11" s="14">
+      <c r="E12" s="14">
         <v>800</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="L12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="M12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="2">
+      <c r="N12" s="2">
         <v>0</v>
       </c>
-      <c r="N11" s="16">
+      <c r="P12" s="16">
         <v>800</v>
       </c>
-      <c r="O11" s="2" t="s">
+      <c r="Q12" s="2" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>